<commit_message>
Complete Cryptocurrency Merkle Tree (M2Q7)
Mistake: merkle tree that minimizes distance to deepest block
</commit_message>
<xml_diff>
--- a/cryptocurrency/inverting_hash_funcs.xlsx
+++ b/cryptocurrency/inverting_hash_funcs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kivanov/Documents/per/bri/cryptocurrency/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EDC1094-5D80-364D-B744-4E1E740C3B79}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7AAC95F-4C01-CD41-8052-8227A352574A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="100" yWindow="460" windowWidth="19200" windowHeight="21320" xr2:uid="{41D8AE72-40DF-CE4E-9B63-1D0066EFCFF7}"/>
   </bookViews>
@@ -423,7 +423,7 @@
   <dimension ref="B6:K43"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B2" zoomScale="125" workbookViewId="0">
-      <selection activeCell="K26" sqref="K26"/>
+      <selection activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -501,8 +501,8 @@
         <v>8</v>
       </c>
       <c r="K11">
-        <f>MOD(J11=H11*7,$I$7)</f>
-        <v>0</v>
+        <f>MOD(J11-H11*7,$I$7)</f>
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="2:11" x14ac:dyDescent="0.2">
@@ -532,8 +532,8 @@
         <v>23</v>
       </c>
       <c r="K12">
-        <f t="shared" ref="K12:K19" si="4">MOD(J12=H12*7,$I$7)</f>
-        <v>0</v>
+        <f t="shared" ref="K12:K19" si="4">MOD(J12-H12*7,$I$7)</f>
+        <v>2</v>
       </c>
     </row>
     <row r="13" spans="2:11" x14ac:dyDescent="0.2">
@@ -564,7 +564,7 @@
       </c>
       <c r="K13">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="14" spans="2:11" x14ac:dyDescent="0.2">
@@ -595,7 +595,7 @@
       </c>
       <c r="K14">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>45</v>
       </c>
     </row>
     <row r="15" spans="2:11" x14ac:dyDescent="0.2">
@@ -626,7 +626,7 @@
       </c>
       <c r="K15">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>99</v>
       </c>
     </row>
     <row r="16" spans="2:11" x14ac:dyDescent="0.2">
@@ -657,7 +657,7 @@
       </c>
       <c r="K16">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>27</v>
       </c>
     </row>
     <row r="17" spans="2:11" x14ac:dyDescent="0.2">
@@ -688,7 +688,7 @@
       </c>
       <c r="K17">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>123</v>
       </c>
     </row>
     <row r="18" spans="2:11" x14ac:dyDescent="0.2">
@@ -719,7 +719,7 @@
       </c>
       <c r="K18">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>209</v>
       </c>
     </row>
     <row r="19" spans="2:11" x14ac:dyDescent="0.2">
@@ -750,7 +750,7 @@
       </c>
       <c r="K19">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>221</v>
       </c>
     </row>
     <row r="20" spans="2:11" x14ac:dyDescent="0.2">

</xml_diff>